<commit_message>
Inserção de produtos e mais
Product's insertion have been finished
Image's thumb changed
Inserting email for newsletter

**************************
Populate categories' menu
Tests and enhancement
</commit_message>
<xml_diff>
--- a/TODOS.xlsx
+++ b/TODOS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="15480" windowHeight="7935"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Produto!$A$1:$P$44</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -189,30 +189,6 @@
           </rPr>
           <t xml:space="preserve">
 Falta Off white</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A34" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>fabianoabreu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta Tamanhos</t>
         </r>
       </text>
     </comment>
@@ -1439,8 +1415,8 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2999,464 +2975,464 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
-      <c r="A35">
+    <row r="35" spans="1:16" s="8" customFormat="1">
+      <c r="A35" s="8">
         <v>8488</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="8">
         <v>110</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="8">
         <v>69.900000000000006</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="K35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L35" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="K35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M35" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
-      <c r="A36">
+    <row r="36" spans="1:16" s="8" customFormat="1">
+      <c r="A36" s="8">
         <v>6622</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="8">
         <v>250</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="K36" t="s">
-        <v>11</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="K36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O36" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
-      <c r="A37">
+    <row r="37" spans="1:16" s="8" customFormat="1">
+      <c r="A37" s="8">
         <v>80101739</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="8">
         <v>239.9</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="8">
         <v>144</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K37" t="s">
-        <v>11</v>
-      </c>
-      <c r="L37" t="s">
-        <v>11</v>
-      </c>
-      <c r="M37" t="s">
+      <c r="K37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="8" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
-      <c r="A38">
+    <row r="38" spans="1:16" s="8" customFormat="1">
+      <c r="A38" s="8">
         <v>350367</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="8">
         <v>210</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="K38" t="s">
-        <v>11</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="K38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="O38" t="s">
+      <c r="O38" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P38" s="8" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
-      <c r="A39">
+    <row r="39" spans="1:16" s="8" customFormat="1">
+      <c r="A39" s="8">
         <v>350362</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="8">
         <v>220</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="K39" t="s">
-        <v>11</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="K39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M39" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O39" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P39" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
-      <c r="A40">
+    <row r="40" spans="1:16" s="8" customFormat="1">
+      <c r="A40" s="8">
         <v>80101820</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="8">
         <v>289.89999999999998</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="8">
         <v>174</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K40" t="s">
-        <v>11</v>
-      </c>
-      <c r="L40" t="s">
-        <v>11</v>
-      </c>
-      <c r="M40" t="s">
+      <c r="K40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M40" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O40" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="P40" t="s">
+      <c r="P40" s="8" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
-      <c r="A41">
+    <row r="41" spans="1:16" s="8" customFormat="1">
+      <c r="A41" s="8">
         <v>80101821</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="8">
         <v>219.9</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="8">
         <v>132</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K41" t="s">
-        <v>11</v>
-      </c>
-      <c r="L41" t="s">
-        <v>11</v>
-      </c>
-      <c r="M41" t="s">
+      <c r="K41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M41" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O41" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" s="8" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
-      <c r="A42">
+    <row r="42" spans="1:16" s="8" customFormat="1">
+      <c r="A42" s="8">
         <v>80201560</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="8">
         <v>289.89999999999998</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="8">
         <v>174</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K42" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42" t="s">
-        <v>11</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="K42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M42" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="O42" t="s">
+      <c r="O42" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P42" s="8" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
-      <c r="A43">
+    <row r="43" spans="1:16" s="8" customFormat="1">
+      <c r="A43" s="8">
         <v>80201561</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="8">
         <v>219.9</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="8">
         <v>132</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K43" t="s">
-        <v>11</v>
-      </c>
-      <c r="L43" t="s">
-        <v>11</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="K43" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O43" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="8" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
-      <c r="A44">
+    <row r="44" spans="1:16" s="8" customFormat="1">
+      <c r="A44" s="8">
         <v>80101845</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="8">
         <v>219.9</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="8">
         <v>132</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K44" t="s">
-        <v>11</v>
-      </c>
-      <c r="L44" t="s">
-        <v>11</v>
-      </c>
-      <c r="M44" t="s">
+      <c r="K44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M44" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N44" t="s">
+      <c r="N44" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="O44" t="s">
+      <c r="O44" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="8" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>

<commit_message>
categorias no menu, optizando imagens...
</commit_message>
<xml_diff>
--- a/TODOS.xlsx
+++ b/TODOS.xlsx
@@ -45,6 +45,30 @@
           </rPr>
           <t xml:space="preserve">
 SEM IMAGEM</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fabiano de Lima Abre:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Questionar sobre foto ser de calça de mulher</t>
         </r>
       </text>
     </comment>
@@ -116,7 +140,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Falta iagem de cor</t>
+Falta iagem de cor Preta</t>
         </r>
       </text>
     </comment>
@@ -1412,11 +1436,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1483,7 +1508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="8" customFormat="1">
+    <row r="2" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A2" s="11">
         <v>10103126</v>
       </c>
@@ -1530,7 +1555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="8" customFormat="1">
+    <row r="3" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A3" s="8">
         <v>80101743</v>
       </c>
@@ -1577,7 +1602,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="8" customFormat="1">
+    <row r="4" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A4" s="8">
         <v>80100727</v>
       </c>
@@ -1624,7 +1649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="8" customFormat="1">
+    <row r="5" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A5" s="14">
         <v>80100552</v>
       </c>
@@ -1671,7 +1696,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1">
+    <row r="6" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A6" s="8">
         <v>10103461</v>
       </c>
@@ -1718,7 +1743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="15" customFormat="1">
+    <row r="7" spans="1:16" s="15" customFormat="1" hidden="1">
       <c r="A7" s="15">
         <v>10103185</v>
       </c>
@@ -1765,7 +1790,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1">
+    <row r="8" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A8" s="8">
         <v>10203288</v>
       </c>
@@ -1812,7 +1837,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="8" customFormat="1">
+    <row r="9" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A9" s="8">
         <v>10201816</v>
       </c>
@@ -1859,51 +1884,51 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="8" customFormat="1">
-      <c r="A10" s="8">
+    <row r="10" spans="1:16" s="10" customFormat="1" hidden="1">
+      <c r="A10" s="10">
         <v>238395</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="10">
         <v>130</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="8" t="s">
+      <c r="K10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="8" customFormat="1">
+    <row r="11" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A11" s="11">
         <v>80201474</v>
       </c>
@@ -1950,7 +1975,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="8" customFormat="1">
+    <row r="12" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A12" s="8">
         <v>80201602</v>
       </c>
@@ -1997,7 +2022,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="8" customFormat="1">
+    <row r="13" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A13" s="8">
         <v>80100438</v>
       </c>
@@ -2044,7 +2069,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="8" customFormat="1">
+    <row r="14" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A14" s="14">
         <v>80200380</v>
       </c>
@@ -2091,7 +2116,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="8" customFormat="1">
+    <row r="15" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A15" s="8">
         <v>10102752</v>
       </c>
@@ -2138,7 +2163,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="8" customFormat="1">
+    <row r="16" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A16" s="8">
         <v>10104784</v>
       </c>
@@ -2185,7 +2210,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="8" customFormat="1">
+    <row r="17" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A17" s="8">
         <v>10103344</v>
       </c>
@@ -2232,7 +2257,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="8" customFormat="1">
+    <row r="18" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A18" s="8">
         <v>10104553</v>
       </c>
@@ -2279,7 +2304,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="8" customFormat="1">
+    <row r="19" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A19" s="8">
         <v>9906</v>
       </c>
@@ -2323,7 +2348,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="8" customFormat="1">
+    <row r="20" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A20" s="8">
         <v>238191</v>
       </c>
@@ -2367,7 +2392,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="8" customFormat="1">
+    <row r="21" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A21" s="11">
         <v>239099</v>
       </c>
@@ -2409,7 +2434,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="10" customFormat="1">
+    <row r="22" spans="1:16" s="10" customFormat="1" hidden="1">
       <c r="A22" s="10">
         <v>5620</v>
       </c>
@@ -2453,7 +2478,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="10" customFormat="1">
+    <row r="23" spans="1:16" s="10" customFormat="1" hidden="1">
       <c r="A23" s="10">
         <v>5613</v>
       </c>
@@ -2541,7 +2566,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="8" customFormat="1">
+    <row r="25" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A25" s="8">
         <v>175051</v>
       </c>
@@ -2585,7 +2610,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="8" customFormat="1">
+    <row r="26" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A26" s="8">
         <v>43022</v>
       </c>
@@ -2755,7 +2780,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="10" customFormat="1">
+    <row r="30" spans="1:16" s="10" customFormat="1" hidden="1">
       <c r="A30" s="10">
         <v>737</v>
       </c>
@@ -2799,7 +2824,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="8" customFormat="1">
+    <row r="31" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A31" s="11">
         <v>6015</v>
       </c>
@@ -2846,7 +2871,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="8" customFormat="1">
+    <row r="32" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A32" s="8">
         <v>238167</v>
       </c>
@@ -2890,7 +2915,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="8" customFormat="1">
+    <row r="33" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A33" s="8">
         <v>237547</v>
       </c>
@@ -2931,7 +2956,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="8" customFormat="1">
+    <row r="34" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A34" s="14">
         <v>1342</v>
       </c>
@@ -2975,7 +3000,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="8" customFormat="1">
+    <row r="35" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A35" s="8">
         <v>8488</v>
       </c>
@@ -3022,7 +3047,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="8" customFormat="1">
+    <row r="36" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A36" s="8">
         <v>6622</v>
       </c>
@@ -3066,7 +3091,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="8" customFormat="1">
+    <row r="37" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A37" s="8">
         <v>80101739</v>
       </c>
@@ -3113,7 +3138,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="8" customFormat="1">
+    <row r="38" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A38" s="8">
         <v>350367</v>
       </c>
@@ -3157,7 +3182,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="8" customFormat="1">
+    <row r="39" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A39" s="8">
         <v>350362</v>
       </c>
@@ -3201,7 +3226,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="8" customFormat="1">
+    <row r="40" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A40" s="8">
         <v>80101820</v>
       </c>
@@ -3248,7 +3273,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="8" customFormat="1">
+    <row r="41" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A41" s="8">
         <v>80101821</v>
       </c>
@@ -3295,7 +3320,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="8" customFormat="1">
+    <row r="42" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A42" s="8">
         <v>80201560</v>
       </c>
@@ -3342,7 +3367,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="8" customFormat="1">
+    <row r="43" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A43" s="8">
         <v>80201561</v>
       </c>
@@ -3389,7 +3414,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="8" customFormat="1">
+    <row r="44" spans="1:16" s="8" customFormat="1" hidden="1">
       <c r="A44" s="8">
         <v>80101845</v>
       </c>
@@ -3437,7 +3462,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P44"/>
+  <autoFilter ref="A1:P44">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="feminino"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="blusas"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Envio de email, mudança de banner
</commit_message>
<xml_diff>
--- a/TODOS.xlsx
+++ b/TODOS.xlsx
@@ -21,33 +21,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Fabiano de Lima Abre</author>
-    <author>fabianoabreu</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Fabiano de Lima Abre:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-SEM IMAGEM</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A10" authorId="0">
       <text>
         <r>
@@ -72,156 +47,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Fabiano de Lima Abre:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta foto das demais cores</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Fabiano de Lima Abre:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Faltando imagem das cores</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Fabiano de Lima Abre:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta iagem de cor Preta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A27" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>fabianoabreu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta cor preta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>fabianoabreu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta preta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A30" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>fabianoabreu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta Off white</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="231">
   <si>
     <t>Codigo do produto (SKU)</t>
   </si>
@@ -702,9 +533,6 @@
   </si>
   <si>
     <t>blusa renda gravatinha ayona</t>
-  </si>
-  <si>
-    <t>cropped gota</t>
   </si>
   <si>
     <t>lacvert</t>
@@ -937,7 +765,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -974,21 +802,8 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1004,12 +819,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1099,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1123,7 +932,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1135,7 +943,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1436,12 +1243,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1452,7 +1258,8 @@
     <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="39" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="88" customWidth="1"/>
@@ -1508,17 +1315,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A2" s="11">
+    <row r="2" spans="1:16" s="8" customFormat="1">
+      <c r="A2" s="10">
         <v>10103126</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>199.9</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>120</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1555,7 +1362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="3" spans="1:16" s="8" customFormat="1">
       <c r="A3" s="8">
         <v>80101743</v>
       </c>
@@ -1602,7 +1409,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="4" spans="1:16" s="8" customFormat="1">
       <c r="A4" s="8">
         <v>80100727</v>
       </c>
@@ -1649,8 +1456,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A5" s="14">
+    <row r="5" spans="1:16" s="8" customFormat="1">
+      <c r="A5" s="13">
         <v>80100552</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1696,7 +1503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="6" spans="1:16" s="8" customFormat="1">
       <c r="A6" s="8">
         <v>10103461</v>
       </c>
@@ -1743,54 +1550,54 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="15" customFormat="1" hidden="1">
-      <c r="A7" s="15">
+    <row r="7" spans="1:16" s="8" customFormat="1">
+      <c r="A7" s="8">
         <v>10103185</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="8">
         <v>189.9</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="8">
         <v>114</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="15" t="s">
+      <c r="K7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="8" spans="1:16" s="8" customFormat="1">
       <c r="A8" s="8">
         <v>10203288</v>
       </c>
@@ -1837,7 +1644,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="9" spans="1:16" s="8" customFormat="1">
       <c r="A9" s="8">
         <v>10201816</v>
       </c>
@@ -1884,61 +1691,61 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="10" customFormat="1" hidden="1">
-      <c r="A10" s="10">
+    <row r="10" spans="1:16" s="9" customFormat="1">
+      <c r="A10" s="9">
         <v>238395</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>130</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="10" t="s">
+      <c r="K10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A11" s="11">
+    <row r="11" spans="1:16" s="8" customFormat="1">
+      <c r="A11" s="10">
         <v>80201474</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>139.9</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>84</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1975,7 +1782,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="12" spans="1:16" s="8" customFormat="1">
       <c r="A12" s="8">
         <v>80201602</v>
       </c>
@@ -2022,7 +1829,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="13" spans="1:16" s="8" customFormat="1">
       <c r="A13" s="8">
         <v>80100438</v>
       </c>
@@ -2069,8 +1876,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A14" s="14">
+    <row r="14" spans="1:16" s="8" customFormat="1">
+      <c r="A14" s="13">
         <v>80200380</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -2116,7 +1923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="15" spans="1:16" s="8" customFormat="1">
       <c r="A15" s="8">
         <v>10102752</v>
       </c>
@@ -2163,7 +1970,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="16" spans="1:16" s="8" customFormat="1">
       <c r="A16" s="8">
         <v>10104784</v>
       </c>
@@ -2210,7 +2017,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="17" spans="1:16" s="8" customFormat="1">
       <c r="A17" s="8">
         <v>10103344</v>
       </c>
@@ -2257,7 +2064,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="18" spans="1:16" s="8" customFormat="1">
       <c r="A18" s="8">
         <v>10104553</v>
       </c>
@@ -2304,7 +2111,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="19" spans="1:16" s="8" customFormat="1">
       <c r="A19" s="8">
         <v>9906</v>
       </c>
@@ -2348,7 +2155,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="20" spans="1:16" s="8" customFormat="1">
       <c r="A20" s="8">
         <v>238191</v>
       </c>
@@ -2392,17 +2199,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A21" s="11">
+    <row r="21" spans="1:16" s="8" customFormat="1">
+      <c r="A21" s="10">
         <v>239099</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="12">
         <v>90</v>
       </c>
-      <c r="D21" s="17"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="8" t="s">
         <v>97</v>
       </c>
@@ -2434,139 +2241,139 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="10" customFormat="1" hidden="1">
-      <c r="A22" s="10">
+    <row r="22" spans="1:16" s="8" customFormat="1">
+      <c r="A22" s="8">
         <v>5620</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="8">
         <v>50</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="10" t="s">
+      <c r="K22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="M22" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="N22" s="10" t="s">
+      <c r="N22" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="O22" s="10" t="s">
+      <c r="O22" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="P22" s="10" t="s">
+      <c r="P22" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="10" customFormat="1" hidden="1">
-      <c r="A23" s="10">
+    <row r="23" spans="1:16" s="8" customFormat="1">
+      <c r="A23" s="8">
         <v>5613</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="8">
         <v>50</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="10" t="s">
+      <c r="K23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="M23" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="N23" s="10" t="s">
+      <c r="N23" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="10" t="s">
+      <c r="O23" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="P23" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="10" customFormat="1">
-      <c r="A24" s="9">
+    <row r="24" spans="1:16" s="8" customFormat="1">
+      <c r="A24" s="13">
         <v>3888</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="8">
         <v>65</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="K24" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="10" t="s">
+      <c r="K24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="10" t="s">
+      <c r="M24" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="N24" s="10" t="s">
+      <c r="N24" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="O24" s="10" t="s">
+      <c r="O24" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="P24" s="10" t="s">
+      <c r="P24" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="25" spans="1:16" s="8" customFormat="1">
       <c r="A25" s="8">
         <v>175051</v>
       </c>
@@ -2610,7 +2417,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="8" customFormat="1" hidden="1">
+    <row r="26" spans="1:16" s="8" customFormat="1">
       <c r="A26" s="8">
         <v>43022</v>
       </c>
@@ -2654,44 +2461,44 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="10" customFormat="1">
-      <c r="A27" s="10">
+    <row r="27" spans="1:16" s="8" customFormat="1">
+      <c r="A27" s="8">
         <v>7788</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="8">
         <v>80</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="K27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="10" t="s">
+      <c r="K27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M27" s="10" t="s">
+      <c r="M27" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="N27" s="10" t="s">
+      <c r="N27" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="O27" s="10" t="s">
+      <c r="O27" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="P27" s="10" t="s">
+      <c r="P27" s="8" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2736,121 +2543,121 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="10" customFormat="1">
-      <c r="A29" s="10">
+    <row r="29" spans="1:16" s="8" customFormat="1">
+      <c r="A29" s="8">
         <v>5076</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="8">
+        <v>70</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="10">
-        <v>70</v>
-      </c>
-      <c r="E29" s="10" t="s">
+      <c r="G29" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="8" customFormat="1">
+      <c r="A30" s="8">
+        <v>737</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="8">
+        <v>90</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="I29" s="10" t="s">
+      <c r="F30" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K29" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L29" s="10" t="s">
+      <c r="K30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="N29" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="O29" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" s="10" customFormat="1" hidden="1">
-      <c r="A30" s="10">
-        <v>737</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="10">
-        <v>90</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="H30" s="10" t="s">
+      <c r="M30" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="O30" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L30" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="N30" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="O30" s="10" t="s">
+      <c r="P30" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="P30" s="10" t="s">
+    </row>
+    <row r="31" spans="1:16" s="8" customFormat="1">
+      <c r="A31" s="10">
+        <v>6015</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A31" s="11">
-        <v>6015</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="C31" s="13">
+      <c r="C31" s="12">
         <v>240</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
         <v>160</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>97</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>14</v>
@@ -2859,24 +2666,24 @@
         <v>11</v>
       </c>
       <c r="M31" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="N31" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="N31" s="8" t="s">
+      <c r="O31" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="O31" s="8" t="s">
+      <c r="P31" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="P31" s="8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="32" spans="1:16" s="8" customFormat="1">
       <c r="A32" s="8">
         <v>238167</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C32" s="8">
         <v>149.9</v>
@@ -2891,10 +2698,10 @@
         <v>149</v>
       </c>
       <c r="H32" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I32" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="K32" s="8" t="s">
         <v>11</v>
@@ -2909,18 +2716,18 @@
         <v>118</v>
       </c>
       <c r="O32" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="P32" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="P32" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="33" spans="1:16" s="8" customFormat="1">
       <c r="A33" s="8">
         <v>237547</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C33" s="8">
         <v>149.9</v>
@@ -2935,7 +2742,7 @@
         <v>21</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>117</v>
@@ -2947,21 +2754,21 @@
         <v>117</v>
       </c>
       <c r="N33" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="O33" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="O33" s="8" t="s">
+      <c r="P33" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="P33" s="8" t="s">
+    </row>
+    <row r="34" spans="1:16" s="8" customFormat="1">
+      <c r="A34" s="13">
+        <v>1342</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" s="8" customFormat="1" hidden="1">
-      <c r="A34" s="14">
-        <v>1342</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="C34" s="8">
         <v>140</v>
@@ -2970,13 +2777,13 @@
         <v>109</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>73</v>
@@ -2988,24 +2795,24 @@
         <v>14</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N34" s="8" t="s">
         <v>128</v>
       </c>
       <c r="O34" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="P34" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="P34" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="35" spans="1:16" s="8" customFormat="1">
       <c r="A35" s="8">
         <v>8488</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35" s="8">
         <v>110</v>
@@ -3017,42 +2824,42 @@
         <v>97</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I35" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M35" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="N35" s="8" t="s">
         <v>128</v>
       </c>
       <c r="O35" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="P35" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="P35" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="36" spans="1:16" s="8" customFormat="1">
       <c r="A36" s="8">
         <v>6622</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C36" s="8">
         <v>250</v>
@@ -3061,16 +2868,16 @@
         <v>30</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H36" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>11</v>
@@ -3082,21 +2889,21 @@
         <v>41</v>
       </c>
       <c r="N36" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="O36" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="O36" s="8" t="s">
+      <c r="P36" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="P36" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="37" spans="1:16" s="8" customFormat="1">
       <c r="A37" s="8">
         <v>80101739</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" s="8">
         <v>239.9</v>
@@ -3114,10 +2921,10 @@
         <v>39</v>
       </c>
       <c r="H37" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>11</v>
@@ -3129,21 +2936,21 @@
         <v>34</v>
       </c>
       <c r="N37" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="O37" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="O37" s="8" t="s">
+      <c r="P37" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="P37" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="38" spans="1:16" s="8" customFormat="1">
       <c r="A38" s="8">
         <v>350367</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C38" s="8">
         <v>210</v>
@@ -3152,16 +2959,16 @@
         <v>97</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K38" s="8" t="s">
         <v>11</v>
@@ -3170,24 +2977,24 @@
         <v>14</v>
       </c>
       <c r="M38" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="O38" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="N38" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="O38" s="8" t="s">
+      <c r="P38" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="P38" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="39" spans="1:16" s="8" customFormat="1">
       <c r="A39" s="8">
         <v>350362</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C39" s="8">
         <v>220</v>
@@ -3196,16 +3003,16 @@
         <v>97</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>11</v>
@@ -3217,21 +3024,21 @@
         <v>158</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" s="8" customFormat="1" hidden="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="8" customFormat="1">
       <c r="A40" s="8">
         <v>80101820</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C40" s="8">
         <v>289.89999999999998</v>
@@ -3246,10 +3053,10 @@
         <v>31</v>
       </c>
       <c r="G40" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H40" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>40</v>
@@ -3264,21 +3071,21 @@
         <v>34</v>
       </c>
       <c r="N40" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="O40" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="O40" s="8" t="s">
+      <c r="P40" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="P40" s="8" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="41" spans="1:16" s="8" customFormat="1">
       <c r="A41" s="8">
         <v>80101821</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C41" s="8">
         <v>219.9</v>
@@ -3293,10 +3100,10 @@
         <v>31</v>
       </c>
       <c r="G41" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H41" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>40</v>
@@ -3311,21 +3118,21 @@
         <v>34</v>
       </c>
       <c r="N41" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="O41" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="O41" s="8" t="s">
+      <c r="P41" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="P41" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="42" spans="1:16" s="8" customFormat="1">
       <c r="A42" s="8">
         <v>80201560</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C42" s="8">
         <v>289.89999999999998</v>
@@ -3340,10 +3147,10 @@
         <v>70</v>
       </c>
       <c r="G42" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>40</v>
@@ -3358,21 +3165,21 @@
         <v>34</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O42" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="P42" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="P42" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="43" spans="1:16" s="8" customFormat="1">
       <c r="A43" s="8">
         <v>80201561</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C43" s="8">
         <v>219.9</v>
@@ -3387,10 +3194,10 @@
         <v>70</v>
       </c>
       <c r="G43" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H43" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>40</v>
@@ -3405,21 +3212,21 @@
         <v>34</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O43" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="P43" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="P43" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" s="8" customFormat="1" hidden="1">
+    </row>
+    <row r="44" spans="1:16" s="8" customFormat="1">
       <c r="A44" s="8">
         <v>80101845</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C44" s="8">
         <v>219.9</v>
@@ -3434,10 +3241,10 @@
         <v>31</v>
       </c>
       <c r="G44" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>40</v>
@@ -3452,27 +3259,19 @@
         <v>34</v>
       </c>
       <c r="N44" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="O44" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="O44" s="8" t="s">
+      <c r="P44" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="P44" s="8" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:P44">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="feminino"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="blusas"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="4"/>
+    <filterColumn colId="6"/>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>